<commit_message>
updated with basic math formulas
</commit_message>
<xml_diff>
--- a/batch_03/Basic_formulas.xlsx
+++ b/batch_03/Basic_formulas.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8832" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8832"/>
   </bookViews>
   <sheets>
-    <sheet name="Text Functins" sheetId="1" r:id="rId1"/>
-    <sheet name="Logical Functions" sheetId="3" r:id="rId2"/>
-    <sheet name="date and Time Functions" sheetId="2" r:id="rId3"/>
+    <sheet name="Basic Math Formulas" sheetId="4" r:id="rId1"/>
+    <sheet name="Text Functins" sheetId="1" r:id="rId2"/>
+    <sheet name="Logical Functions" sheetId="3" r:id="rId3"/>
+    <sheet name="date and Time Functions" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="144">
   <si>
     <t>CONCATENATE(), TEXT(), LEFT(), RIGHT(), MID(), LEN(), TRIM(), UPPER(), LOWER(), PROPER(), REPT(), SUBSTITUTE(), FIND(), SEARCH()</t>
   </si>
@@ -404,6 +405,60 @@
   </si>
   <si>
     <t>Function Name</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>dsdasdadsa</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>=QUOTIENT()</t>
+  </si>
+  <si>
+    <t>mod()</t>
+  </si>
+  <si>
+    <t>multiplication | Product</t>
+  </si>
+  <si>
+    <t>count()</t>
+  </si>
+  <si>
+    <t>counta()</t>
+  </si>
+  <si>
+    <t>=LEN(A2)</t>
+  </si>
+  <si>
+    <t>power()</t>
+  </si>
+  <si>
+    <t>sqrt()</t>
+  </si>
+  <si>
+    <t>round()</t>
+  </si>
+  <si>
+    <t>celing()</t>
+  </si>
+  <si>
+    <t>roundup()</t>
+  </si>
+  <si>
+    <t>rand()</t>
+  </si>
+  <si>
+    <t>randbetween()</t>
+  </si>
+  <si>
+    <t>lower()</t>
   </si>
 </sst>
 </file>
@@ -495,7 +550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -536,6 +591,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -817,10 +875,1093 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" t="s">
+        <v>133</v>
+      </c>
+      <c r="J1" t="s">
+        <v>134</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" t="s">
+        <v>136</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="N1" t="s">
+        <v>138</v>
+      </c>
+      <c r="O1" t="s">
+        <v>139</v>
+      </c>
+      <c r="P1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="R1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" s="12">
+        <v>333</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>SUM(A2:B2)</f>
+        <v>333</v>
+      </c>
+      <c r="D2">
+        <f>A2*B2</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>PRODUCT(A2:B2)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" t="e">
+        <f>QUOTIENT(A2,B2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G2" t="e">
+        <f>MOD(A2,B2)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H2">
+        <f>AVERAGE(A2:B2)</f>
+        <v>166.5</v>
+      </c>
+      <c r="I2">
+        <f>COUNT(A2:B2)</f>
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <f>COUNTA(A2:B2)</f>
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K16" si="0">LEN(A3)</f>
+        <v>3</v>
+      </c>
+      <c r="L2">
+        <f>POWER(2,2)</f>
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <f>SQRT(A2)</f>
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N2">
+        <f>ROUND(M2,2)</f>
+        <v>18.25</v>
+      </c>
+      <c r="O2">
+        <f>CEILING(M2,1)</f>
+        <v>19</v>
+      </c>
+      <c r="P2">
+        <f>ROUNDUP(M2,0)</f>
+        <v>19</v>
+      </c>
+      <c r="Q2">
+        <f ca="1">RAND()</f>
+        <v>0.50632973014391169</v>
+      </c>
+      <c r="R2">
+        <f ca="1">RANDBETWEEN(100,1000)</f>
+        <v>979</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" s="12">
+        <v>333</v>
+      </c>
+      <c r="B3" s="12">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C6" si="1">SUM(A3:B3)</f>
+        <v>358</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="2">A3*B3</f>
+        <v>8325</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E15" si="3">PRODUCT(A3:B3)</f>
+        <v>8325</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F15" si="4">QUOTIENT(A3,B3)</f>
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <f>MOD(A3,B3)</f>
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <f>AVERAGE(A3:B3)</f>
+        <v>179</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I15" si="5">COUNT(A3:B3)</f>
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J16" si="6">COUNTA(A3:B3)</f>
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <f>POWER(A3,3)</f>
+        <v>36926037</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M16" si="7">SQRT(A3)</f>
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N3">
+        <f>ROUND(M3,3)</f>
+        <v>18.248000000000001</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O16" si="8">CEILING(M3,1)</f>
+        <v>19</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P16" si="9">ROUNDUP(M3,0)</f>
+        <v>19</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q16" ca="1" si="10">RAND()</f>
+        <v>0.5459949798527699</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R16" ca="1" si="11">RANDBETWEEN(100,1000)</f>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
+        <v>333</v>
+      </c>
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>333</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F4" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G4" t="e">
+        <f>MOD(A4,B4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H4">
+        <f>AVERAGE(A4:B4)</f>
+        <v>166.5</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L16" si="12">POWER(A4,3)</f>
+        <v>36926037</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="7"/>
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N3:N16" si="13">ROUND(M4,2)</f>
+        <v>18.25</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.88000406943361442</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ca="1" si="11"/>
+        <v>820</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>333</v>
+      </c>
+      <c r="B5" s="12">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>378</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>14985</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>14985</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <f>MOD(A5,B5)</f>
+        <v>18</v>
+      </c>
+      <c r="H5">
+        <f>AVERAGE(A5:B5)</f>
+        <v>189</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="12"/>
+        <v>36926037</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="7"/>
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N5">
+        <f>ROUND(M5,0)</f>
+        <v>18</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.77941354805640017</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ca="1" si="11"/>
+        <v>897</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>333</v>
+      </c>
+      <c r="B6" s="12">
+        <v>55</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>388</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>18315</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>18315</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <f>MOD(A6,B6)</f>
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <f>AVERAGE(A6:B6)</f>
+        <v>194</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="12"/>
+        <v>36926037</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="7"/>
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="13"/>
+        <v>18.25</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.95250145064686631</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ca="1" si="11"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3333</v>
+      </c>
+      <c r="B7">
+        <f>SUM(B2:B6)</f>
+        <v>125</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C2:C6)</f>
+        <v>1790</v>
+      </c>
+      <c r="D7">
+        <f>SUM(D2:D6)</f>
+        <v>41625</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>416625</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="G7">
+        <f>MOD(A7,B7)</f>
+        <v>83</v>
+      </c>
+      <c r="H7">
+        <f>AVERAGE(A7:B7)</f>
+        <v>1729</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="12"/>
+        <v>37025927037</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="7"/>
+        <v>57.732140095444237</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="13"/>
+        <v>57.73</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="8"/>
+        <v>58</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="9"/>
+        <v>58</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.65708508319933712</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ca="1" si="11"/>
+        <v>776</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>AVERAGE(A2:A7)</f>
+        <v>833</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(B2:B7)</f>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(C2:C7)</f>
+        <v>596.66666666666663</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(D2:D7)</f>
+        <v>13875</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>34708.333333333328</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="G8">
+        <f>MOD(A8,B8)</f>
+        <v>41.333333333333378</v>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(A8:B8)</f>
+        <v>437.33333333333331</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="12"/>
+        <v>578009537</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="7"/>
+        <v>28.861739379323623</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="13"/>
+        <v>28.86</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="8"/>
+        <v>29</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="9"/>
+        <v>29</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" ca="1" si="10"/>
+        <v>3.8214141102763555E-2</v>
+      </c>
+      <c r="R8">
+        <f t="shared" ca="1" si="11"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>MAX(A2:A8)</f>
+        <v>3333</v>
+      </c>
+      <c r="B9">
+        <f>MAX(B2:B8)</f>
+        <v>125</v>
+      </c>
+      <c r="C9">
+        <f>MAX(C2:C8)</f>
+        <v>1790</v>
+      </c>
+      <c r="D9">
+        <f>MAX(D2:D8)</f>
+        <v>41625</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>416625</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="G9">
+        <f>MOD(A9,B9)</f>
+        <v>83</v>
+      </c>
+      <c r="H9">
+        <f>AVERAGE(A9:B9)</f>
+        <v>1729</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="12"/>
+        <v>37025927037</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="7"/>
+        <v>57.732140095444237</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="13"/>
+        <v>57.73</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="8"/>
+        <v>58</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="9"/>
+        <v>58</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.86664837765366554</v>
+      </c>
+      <c r="R9">
+        <f t="shared" ca="1" si="11"/>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f>MIN(A2:A9)</f>
+        <v>333</v>
+      </c>
+      <c r="B10">
+        <f>MIN(B2:B9)</f>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>MIN(C2:C9)</f>
+        <v>333</v>
+      </c>
+      <c r="D10">
+        <f>MIN(D2:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F10" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10" t="e">
+        <f>MOD(A10,B10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10">
+        <f>AVERAGE(A10:B10)</f>
+        <v>166.5</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="12"/>
+        <v>36926037</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="7"/>
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="13"/>
+        <v>18.25</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ca="1" si="10"/>
+        <v>6.9391017796488041E-2</v>
+      </c>
+      <c r="R10">
+        <f t="shared" ca="1" si="11"/>
+        <v>383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f>COUNT(A2:A10)</f>
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f>COUNT(B2:B10)</f>
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <f>COUNT(C2:C10)</f>
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <f>COUNT(D2:D10)</f>
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>81</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <f>MOD(A11,B11)</f>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f>AVERAGE(A11:B11)</f>
+        <v>9</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="12"/>
+        <v>729</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="7"/>
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="13"/>
+        <v>3</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.73962373740332221</v>
+      </c>
+      <c r="R11">
+        <f t="shared" ca="1" si="11"/>
+        <v>815</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F12" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" t="e">
+        <f>MOD(A12,B12)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H12">
+        <v>33</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.84440651673871248</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ca="1" si="11"/>
+        <v>564</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F13" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G13">
+        <v>33</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f>COUNTA(A13:B13)</f>
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L13" t="e">
+        <f t="shared" si="12"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M13" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N13" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O13" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P13" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.40920873847735018</v>
+      </c>
+      <c r="R13">
+        <f t="shared" ca="1" si="11"/>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="F14" t="e">
+        <f>QUOTIENT(A14,B14)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14">
+        <v>33</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="7"/>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="13"/>
+        <v>1.41</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.32406762635350828</v>
+      </c>
+      <c r="R14">
+        <f t="shared" ca="1" si="11"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F15" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15">
+        <v>33</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.8687194688636376</v>
+      </c>
+      <c r="R15">
+        <f t="shared" ca="1" si="11"/>
+        <v>602</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <f>PRODUCT(A16:B16)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" t="e">
+        <f>QUOTIENT(A16,B16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H16">
+        <v>33</v>
+      </c>
+      <c r="I16">
+        <f>COUNT(A16:B16)</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" ca="1" si="10"/>
+        <v>0.25067842953879249</v>
+      </c>
+      <c r="R16">
+        <f t="shared" ca="1" si="11"/>
+        <v>583</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC34"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:L5"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -833,11 +1974,20 @@
     <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.5546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.88671875" customWidth="1"/>
-    <col min="23" max="23" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="8.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -961,6 +2111,9 @@
       <c r="S3" t="s">
         <v>69</v>
       </c>
+      <c r="T3" t="s">
+        <v>143</v>
+      </c>
       <c r="U3" t="s">
         <v>70</v>
       </c>
@@ -1009,8 +2162,8 @@
         <v>548.97149999999999</v>
       </c>
       <c r="K4" t="str">
-        <f>CONCATENATE(D4,"Trichy")</f>
-        <v>MemberTrichy</v>
+        <f>CONCATENATE(D4,"_",C4)</f>
+        <v>Member_Trichy</v>
       </c>
       <c r="L4" t="str">
         <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
@@ -1040,13 +2193,17 @@
         <f>UPPER(F4)</f>
         <v xml:space="preserve"> HEALTH AND BEAUTY </v>
       </c>
+      <c r="T4" t="str">
+        <f>LOWER(F4)</f>
+        <v xml:space="preserve"> health and beauty </v>
+      </c>
       <c r="U4" t="str">
         <f>PROPER(F4)</f>
         <v xml:space="preserve"> Health And Beauty </v>
       </c>
       <c r="V4" t="str">
-        <f>REPT(H4,5)</f>
-        <v>77777</v>
+        <f>REPT(P4,2)</f>
+        <v>1919</v>
       </c>
       <c r="W4" t="str">
         <f ca="1">SUBSTITUTE(L4,"/","-")</f>
@@ -1054,7 +2211,7 @@
       </c>
       <c r="X4">
         <f>FIND("Trichy",K4)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Y4">
         <f>SEARCH("Member",K4)</f>
@@ -1093,8 +2250,8 @@
         <v>80.22</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5:K34" si="0">CONCATENATE(C5,"_",D5)</f>
-        <v>Chennai_Normal</v>
+        <f>CONCATENATE(C5,"_",D5,"_")</f>
+        <v>Chennai_Normal_</v>
       </c>
       <c r="L5" t="str">
         <f>TEXT("20/13/2020","mm/dd/yyyy")</f>
@@ -1105,11 +2262,11 @@
         <v>17</v>
       </c>
       <c r="X5" t="e">
-        <f t="shared" ref="X5:X8" si="1">FIND("Trichy",K5)</f>
+        <f t="shared" ref="X5:X8" si="0">FIND("Trichy",K5)</f>
         <v>#VALUE!</v>
       </c>
       <c r="Y5" t="e">
-        <f t="shared" ref="Y5:Y23" si="2">SEARCH("Member",K5)</f>
+        <f t="shared" ref="Y5:Y23" si="1">SEARCH("Member",K5)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1145,15 +2302,15 @@
         <v>340.52550000000002</v>
       </c>
       <c r="K6" t="str">
+        <f t="shared" ref="K5:K34" si="2">CONCATENATE(C6,"_",D6)</f>
+        <v>Trichy_Normal</v>
+      </c>
+      <c r="X6">
         <f t="shared" si="0"/>
-        <v>Trichy_Normal</v>
-      </c>
-      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="e">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y6" t="e">
-        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1189,7 +2346,7 @@
         <v>489.048</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Member</v>
       </c>
       <c r="L7" s="3">
@@ -1197,11 +2354,11 @@
         <v>45694</v>
       </c>
       <c r="X7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Y7">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y7">
-        <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
@@ -1237,15 +2394,15 @@
         <v>634.37850000000003</v>
       </c>
       <c r="K8" t="str">
+        <f t="shared" si="2"/>
+        <v>Trichy_Normal</v>
+      </c>
+      <c r="X8">
         <f t="shared" si="0"/>
-        <v>Trichy_Normal</v>
-      </c>
-      <c r="X8">
+        <v>1</v>
+      </c>
+      <c r="Y8" t="e">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Y8" t="e">
-        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1281,11 +2438,11 @@
         <v>627.61649999999997</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Chennai_Normal</v>
       </c>
       <c r="Y9" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1321,11 +2478,11 @@
         <v>433.69200000000001</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Member</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -1361,11 +2518,11 @@
         <v>772.38</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Chennai_Normal</v>
       </c>
       <c r="Y11" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1401,11 +2558,11 @@
         <v>76.146000000000001</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Member</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -1441,11 +2598,11 @@
         <v>172.74600000000001</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>karur_Member</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -1481,11 +2638,11 @@
         <v>60.816000000000003</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>karur_Member</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -1521,11 +2678,11 @@
         <v>107.142</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>karur_Member</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -1561,11 +2718,11 @@
         <v>246.48750000000001</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Normal</v>
       </c>
       <c r="Y16" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1601,11 +2758,11 @@
         <v>453.495</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Normal</v>
       </c>
       <c r="Y17" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1641,11 +2798,11 @@
         <v>749.49</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Normal</v>
       </c>
       <c r="Y18" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1681,11 +2838,11 @@
         <v>590.43600000000004</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>karur_Member</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
@@ -1721,11 +2878,11 @@
         <v>506.63549999999998</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Member</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
@@ -1761,11 +2918,11 @@
         <v>457.44299999999998</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Normal</v>
       </c>
       <c r="Y21" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1801,11 +2958,11 @@
         <v>172.2105</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Normal</v>
       </c>
       <c r="Y22" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1841,11 +2998,11 @@
         <v>84.63</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>karur_Normal</v>
       </c>
       <c r="Y23" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -1881,7 +3038,7 @@
         <v>451.71</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Chennai_Member</v>
       </c>
     </row>
@@ -1917,7 +3074,7 @@
         <v>277.137</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>karur_Normal</v>
       </c>
     </row>
@@ -1953,7 +3110,7 @@
         <v>69.72</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>karur_Normal</v>
       </c>
     </row>
@@ -1989,7 +3146,7 @@
         <v>181.44</v>
       </c>
       <c r="K27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Normal</v>
       </c>
     </row>
@@ -2025,7 +3182,7 @@
         <v>279.18450000000001</v>
       </c>
       <c r="K28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Member</v>
       </c>
     </row>
@@ -2061,7 +3218,7 @@
         <v>441.75599999999997</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Member</v>
       </c>
     </row>
@@ -2097,7 +3254,7 @@
         <v>35.195999999999998</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>karur_Normal</v>
       </c>
     </row>
@@ -2133,7 +3290,7 @@
         <v>184.107</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Normal</v>
       </c>
     </row>
@@ -2169,7 +3326,7 @@
         <v>463.89</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>karur_Normal</v>
       </c>
     </row>
@@ -2205,7 +3362,7 @@
         <v>235.2105</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>Trichy_Normal</v>
       </c>
     </row>
@@ -2241,7 +3398,7 @@
         <v>494.1825</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>karur_Normal</v>
       </c>
     </row>
@@ -2255,15 +3412,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q10" sqref="A1:Q10"/>
+      <selection pane="bottomRight" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2773,19 +3930,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
@@ -2893,15 +4049,15 @@
       </c>
       <c r="E5" s="4">
         <f ca="1">NOW()</f>
-        <v>45694.462209143516</v>
+        <v>45694.618251851854</v>
       </c>
       <c r="F5" s="5">
         <f>TIME(2,30,30)</f>
         <v>0.10451388888888889</v>
       </c>
       <c r="G5">
-        <f ca="1">DATEDIF(C5,D5,"Y")</f>
-        <v>4</v>
+        <f ca="1">DATEDIF(C5,D5,"ym")</f>
+        <v>1</v>
       </c>
       <c r="H5">
         <f ca="1">YEAR(D5)</f>
@@ -2913,15 +4069,27 @@
       </c>
       <c r="J5">
         <f ca="1">HOUR(E5)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="K5">
         <f ca="1">MINUTE(E5)</f>
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="L5">
         <f ca="1">SECOND(E5)</f>
-        <v>35</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D10" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D11" s="4">
+        <f ca="1">NOW()</f>
+        <v>45694.618251851854</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added formulas for statistical functions and v and h lookup
</commit_message>
<xml_diff>
--- a/batch_03/Basic_formulas.xlsx
+++ b/batch_03/Basic_formulas.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8832" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8832" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Math Formulas" sheetId="4" r:id="rId1"/>
     <sheet name="Text Functins" sheetId="1" r:id="rId2"/>
     <sheet name="Logical Functions" sheetId="3" r:id="rId3"/>
     <sheet name="date and Time Functions" sheetId="2" r:id="rId4"/>
+    <sheet name="Statistical Functions" sheetId="5" r:id="rId5"/>
+    <sheet name="Lookup (V and H _Lookup) " sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="174">
   <si>
     <t>CONCATENATE(), TEXT(), LEFT(), RIGHT(), MID(), LEN(), TRIM(), UPPER(), LOWER(), PROPER(), REPT(), SUBSTITUTE(), FIND(), SEARCH()</t>
   </si>
@@ -462,13 +464,100 @@
   </si>
   <si>
     <t>12.12.2007</t>
+  </si>
+  <si>
+    <t>AVERAGE(), MEDIAN(), MODE(), COUNT(), COUNTA(), COUNTIF(), COUNTIFS(), MAX(), MIN(), STDEV(), VAR()</t>
+  </si>
+  <si>
+    <t>Statistical Functions</t>
+  </si>
+  <si>
+    <t>VLOOKUP(), HLOOKUP(), LOOKUP()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lookup (V-Lookup and H-Lookup) </t>
+  </si>
+  <si>
+    <t>=MEDIAN(A5:A9)</t>
+  </si>
+  <si>
+    <t>=AVERAGE(A5:A9)</t>
+  </si>
+  <si>
+    <t>=MODE(A5:A9)</t>
+  </si>
+  <si>
+    <t>mode()</t>
+  </si>
+  <si>
+    <t>asending order</t>
+  </si>
+  <si>
+    <t>dataset original</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> after asending pick center value</t>
+  </si>
+  <si>
+    <t>=COUNT(A5:A9)</t>
+  </si>
+  <si>
+    <t>=COUNTA(C5:C9)</t>
+  </si>
+  <si>
+    <t>=COUNTIF(C5:C9,"A")</t>
+  </si>
+  <si>
+    <t>=COUNTIFS(C5:C9,"A",B5:B9,0)</t>
+  </si>
+  <si>
+    <t>=MAX(B5:B9)</t>
+  </si>
+  <si>
+    <t>=MIN(B5:B9)</t>
+  </si>
+  <si>
+    <t>=STDEV(A5:A9)</t>
+  </si>
+  <si>
+    <t>=VAR(A5:A9)</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t>fsd</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Fees Pending</t>
+  </si>
+  <si>
+    <t>=VLOOKUP(G7,A5:F26,2)</t>
+  </si>
+  <si>
+    <t>=HLOOKUP(G7,A16:F26,2,)</t>
+  </si>
+  <si>
+    <t>Exact Match (False)</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,6 +584,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -526,7 +623,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -549,11 +646,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -589,6 +695,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -598,8 +706,28 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,11 +1142,11 @@
       </c>
       <c r="Q2">
         <f ca="1">RAND()</f>
-        <v>0.60394970536282289</v>
+        <v>0.78110030991428259</v>
       </c>
       <c r="R2">
         <f ca="1">RANDBETWEEN(100,1000)</f>
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -1086,11 +1214,11 @@
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q16" ca="1" si="12">RAND()</f>
-        <v>9.0058049699657139E-2</v>
+        <v>0.94561602312717785</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R16" ca="1" si="13">RANDBETWEEN(100,1000)</f>
-        <v>235</v>
+        <v>559</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -1158,11 +1286,11 @@
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="12"/>
-        <v>0.52602215835702615</v>
+        <v>0.48896558051248562</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="13"/>
-        <v>338</v>
+        <v>812</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1230,11 +1358,11 @@
       </c>
       <c r="Q5">
         <f t="shared" ca="1" si="12"/>
-        <v>0.71440632453350739</v>
+        <v>0.98660386632513752</v>
       </c>
       <c r="R5">
         <f t="shared" ca="1" si="13"/>
-        <v>253</v>
+        <v>919</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -1302,11 +1430,11 @@
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="12"/>
-        <v>0.7074465995596706</v>
+        <v>0.80457349761848052</v>
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="13"/>
-        <v>484</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -1375,11 +1503,11 @@
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="12"/>
-        <v>0.1605943939453699</v>
+        <v>0.76339599531035929</v>
       </c>
       <c r="R7">
         <f t="shared" ca="1" si="13"/>
-        <v>137</v>
+        <v>979</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -1449,11 +1577,11 @@
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="12"/>
-        <v>0.83334648399171363</v>
+        <v>0.16880788051704509</v>
       </c>
       <c r="R8">
         <f t="shared" ca="1" si="13"/>
-        <v>595</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -1523,11 +1651,11 @@
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="12"/>
-        <v>0.23785276135270061</v>
+        <v>0.73204195694662977</v>
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="13"/>
-        <v>878</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -1597,11 +1725,11 @@
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="12"/>
-        <v>0.26410365566756044</v>
+        <v>0.8522242868489639</v>
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="13"/>
-        <v>597</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -1671,11 +1799,11 @@
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="12"/>
-        <v>0.89243745821069531</v>
+        <v>0.68442828288013036</v>
       </c>
       <c r="R11">
         <f t="shared" ca="1" si="13"/>
-        <v>217</v>
+        <v>968</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -1728,11 +1856,11 @@
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="12"/>
-        <v>0.65465421741499108</v>
+        <v>0.66244324087640438</v>
       </c>
       <c r="R12">
         <f t="shared" ca="1" si="13"/>
-        <v>234</v>
+        <v>666</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -1787,11 +1915,11 @@
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="12"/>
-        <v>4.8003841425799054E-2</v>
+        <v>0.91636972576779496</v>
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="13"/>
-        <v>145</v>
+        <v>674</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -1843,11 +1971,11 @@
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="12"/>
-        <v>0.88669591518661706</v>
+        <v>0.80965757593807008</v>
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="13"/>
-        <v>396</v>
+        <v>768</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -1896,11 +2024,11 @@
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="12"/>
-        <v>0.45218813419158177</v>
+        <v>0.9841513342958369</v>
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="13"/>
-        <v>873</v>
+        <v>614</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1949,11 +2077,11 @@
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="12"/>
-        <v>0.97703855930663908</v>
+        <v>0.82182337475158085</v>
       </c>
       <c r="R16">
         <f t="shared" ca="1" si="13"/>
-        <v>960</v>
+        <v>714</v>
       </c>
     </row>
   </sheetData>
@@ -1996,57 +2124,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="20"/>
-      <c r="AA1" s="20"/>
-      <c r="AB1" s="20"/>
-      <c r="AC1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
+      <c r="AB1" s="22"/>
+      <c r="AC1" s="22"/>
     </row>
     <row r="2" spans="1:29" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
+      <c r="E2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -2172,7 +2300,7 @@
       </c>
       <c r="L4" t="str">
         <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
-        <v>02/07/2025</v>
+        <v>02/10/2025</v>
       </c>
       <c r="M4" t="str">
         <f>LEFT(F4,5)</f>
@@ -2212,7 +2340,7 @@
       </c>
       <c r="W4" t="str">
         <f ca="1">SUBSTITUTE(L4,"/","-")</f>
-        <v>02-07-2025</v>
+        <v>02-10-2025</v>
       </c>
       <c r="X4">
         <f>FIND("Trichy",K4)</f>
@@ -2356,7 +2484,7 @@
       </c>
       <c r="L7" s="3">
         <f ca="1">TODAY()</f>
-        <v>45695</v>
+        <v>45698</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
@@ -3421,11 +3549,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
+      <selection pane="bottomRight" sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3451,13 +3579,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="23" t="s">
         <v>87</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -3504,9 +3632,9 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="7" t="s">
         <v>99</v>
       </c>
@@ -3551,9 +3679,9 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="9" t="s">
         <v>110</v>
       </c>
@@ -3975,28 +4103,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
@@ -4011,16 +4139,16 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -4067,11 +4195,11 @@
       </c>
       <c r="D5" s="3">
         <f ca="1">TODAY()</f>
-        <v>45695</v>
+        <v>45698</v>
       </c>
       <c r="E5" s="4">
         <f ca="1">NOW()</f>
-        <v>45695.638882638887</v>
+        <v>45698.635017592591</v>
       </c>
       <c r="F5" s="5">
         <f>TIME(2,30,30)</f>
@@ -4079,7 +4207,7 @@
       </c>
       <c r="G5">
         <f ca="1">DATEDIF(C5,D5,"ym")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <f ca="1">YEAR(D5)</f>
@@ -4087,7 +4215,7 @@
       </c>
       <c r="I5">
         <f ca="1">DAY(D5)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J5">
         <f ca="1">HOUR(E5)</f>
@@ -4095,15 +4223,15 @@
       </c>
       <c r="K5">
         <f ca="1">MINUTE(E5)</f>
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L5">
         <f ca="1">SECOND(E5)</f>
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I9" s="23">
+      <c r="I9" s="20">
         <v>12</v>
       </c>
       <c r="J9">
@@ -4123,7 +4251,7 @@
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D10" s="3">
         <f ca="1">TODAY()</f>
-        <v>45695</v>
+        <v>45698</v>
       </c>
       <c r="E10">
         <f ca="1">YEAR(D10)</f>
@@ -4135,9 +4263,9 @@
       </c>
       <c r="G10">
         <f ca="1">YEARFRAC(TODAY(),C5)</f>
-        <v>4.1583333333333332</v>
-      </c>
-      <c r="I10" s="23">
+        <v>4.166666666666667</v>
+      </c>
+      <c r="I10" s="20">
         <v>12</v>
       </c>
       <c r="J10">
@@ -4157,9 +4285,9 @@
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D11" s="4">
         <f ca="1">NOW()</f>
-        <v>45695.638882638887</v>
-      </c>
-      <c r="I11" s="23">
+        <v>45698.635017592591</v>
+      </c>
+      <c r="I11" s="20">
         <v>12</v>
       </c>
       <c r="J11">
@@ -4181,7 +4309,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I12" s="23"/>
+      <c r="I12" s="20"/>
       <c r="L12" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#NUM!</v>
@@ -4191,13 +4319,13 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E13" s="22">
+      <c r="E13" s="19">
         <v>0.61597222222222225</v>
       </c>
       <c r="G13" s="4">
         <v>45695.616666666669</v>
       </c>
-      <c r="I13" s="23">
+      <c r="I13" s="20">
         <v>12</v>
       </c>
       <c r="J13">
@@ -4217,9 +4345,9 @@
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="E14" s="3">
         <f ca="1">TODAY()</f>
-        <v>45695</v>
-      </c>
-      <c r="I14" s="23"/>
+        <v>45698</v>
+      </c>
+      <c r="I14" s="20"/>
       <c r="L14" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#NUM!</v>
@@ -4234,9 +4362,9 @@
       </c>
       <c r="G15" s="4">
         <f ca="1">NOW()</f>
-        <v>45695.638882638887</v>
-      </c>
-      <c r="I15" s="23">
+        <v>45698.635017592591</v>
+      </c>
+      <c r="I15" s="20">
         <v>12</v>
       </c>
       <c r="J15">
@@ -4254,10 +4382,10 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E16" s="22">
+      <c r="E16" s="19">
         <v>0.61597222222222225</v>
       </c>
-      <c r="I16" s="23"/>
+      <c r="I16" s="20"/>
       <c r="L16" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#NUM!</v>
@@ -4267,7 +4395,7 @@
       </c>
     </row>
     <row r="17" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="I17" s="23"/>
+      <c r="I17" s="20"/>
       <c r="L17" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#NUM!</v>
@@ -4280,7 +4408,7 @@
       <c r="E18" s="3">
         <v>45695</v>
       </c>
-      <c r="I18" s="23">
+      <c r="I18" s="20">
         <v>12</v>
       </c>
       <c r="J18">
@@ -4298,7 +4426,7 @@
       </c>
     </row>
     <row r="19" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E19" s="22">
+      <c r="E19" s="19">
         <v>0.61597222222222225</v>
       </c>
       <c r="L19" t="s">
@@ -4309,7 +4437,7 @@
       </c>
     </row>
     <row r="20" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E20" s="22">
+      <c r="E20" s="19">
         <v>0.6166666666666667</v>
       </c>
     </row>
@@ -4320,4 +4448,664 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" customWidth="1"/>
+    <col min="10" max="10" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="J4" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="K4" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>161</v>
+      </c>
+      <c r="M4" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="N4" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="12">
+        <v>44</v>
+      </c>
+      <c r="B5" s="12">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <f>AVERAGE(A5:A9)</f>
+        <v>35.6</v>
+      </c>
+      <c r="E5">
+        <f>MEDIAN(A5:A9)</f>
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <f>MODE(A5:A9)</f>
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <f>COUNT(A5:A9)</f>
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <f>COUNTA(C5:C9)</f>
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <f>COUNTIF(C5:C9,"A")</f>
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <f>COUNTIFS(C5:C9,"A",B5:B9,0)</f>
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <f>MAX(B5:B9)</f>
+        <v>55</v>
+      </c>
+      <c r="L5">
+        <f>MIN(B5:B9)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="24">
+        <f>STDEV(A5:A9)</f>
+        <v>7.6681158050723228</v>
+      </c>
+      <c r="N5">
+        <f>VAR(A5:A9)</f>
+        <v>58.799999999999955</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
+        <v>30</v>
+      </c>
+      <c r="B6" s="12">
+        <v>25</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D9" si="0">AVERAGE(A6:A10)</f>
+        <v>33.5</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E9" si="1">MEDIAN(A6:A10)</f>
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <f>MODE(A5:A10)</f>
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:G9" si="2">COUNT(A6:A10)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>30</v>
+      </c>
+      <c r="B7" s="12">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>34.666666666666664</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="12">
+        <v>30</v>
+      </c>
+      <c r="B8" s="12">
+        <v>45</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="12">
+        <v>44</v>
+      </c>
+      <c r="B9" s="12">
+        <v>55</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="29"/>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <f>MEDIAN(C16:G16)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E2:P2"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B1" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="12">
+        <v>40</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="12">
+        <v>55</v>
+      </c>
+      <c r="C6" s="12">
+        <v>25</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B7" s="12">
+        <v>30</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="31">
+        <f>VLOOKUP(G7,A5:F26,2)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="12">
+        <v>40</v>
+      </c>
+      <c r="C8" s="12">
+        <v>45</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E8" s="12">
+        <v>33</v>
+      </c>
+      <c r="F8" s="12">
+        <v>333</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="31">
+        <f>VLOOKUP(G8,A5:F26,3)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" s="12">
+        <v>50</v>
+      </c>
+      <c r="C9" s="12">
+        <v>55</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G16" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="H16" s="33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="12">
+        <v>40</v>
+      </c>
+      <c r="C17" s="12">
+        <v>55</v>
+      </c>
+      <c r="D17" s="12">
+        <v>30</v>
+      </c>
+      <c r="E17" s="12">
+        <v>40</v>
+      </c>
+      <c r="F17" s="12">
+        <v>50</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="H17" s="32">
+        <f>HLOOKUP(G17,A16:F26,2,)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="B18" s="12">
+        <v>0</v>
+      </c>
+      <c r="C18" s="12">
+        <v>25</v>
+      </c>
+      <c r="D18" s="12">
+        <v>0</v>
+      </c>
+      <c r="E18" s="12">
+        <v>45</v>
+      </c>
+      <c r="F18" s="12">
+        <v>55</v>
+      </c>
+      <c r="G18" s="31">
+        <v>50</v>
+      </c>
+      <c r="H18" s="32">
+        <f>HLOOKUP(G18,B17:F21,2,TRUE)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12">
+        <v>33</v>
+      </c>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12">
+        <v>333</v>
+      </c>
+      <c r="F21" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D2:N2"/>
+    <mergeCell ref="B1:T1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update formula sheet with reference formulas
</commit_message>
<xml_diff>
--- a/batch_03/Basic_formulas.xlsx
+++ b/batch_03/Basic_formulas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8832" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8832" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Math Formulas" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="date and Time Functions" sheetId="2" r:id="rId4"/>
     <sheet name="Statistical Functions" sheetId="5" r:id="rId5"/>
     <sheet name="Lookup (V and H _Lookup) " sheetId="6" r:id="rId6"/>
+    <sheet name="Reference Functions" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="190">
   <si>
     <t>CONCATENATE(), TEXT(), LEFT(), RIGHT(), MID(), LEN(), TRIM(), UPPER(), LOWER(), PROPER(), REPT(), SUBSTITUTE(), FIND(), SEARCH()</t>
   </si>
@@ -412,39 +413,15 @@
     <t>total</t>
   </si>
   <si>
-    <t>dsdasdadsa</t>
-  </si>
-  <si>
     <t>average</t>
   </si>
   <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>=QUOTIENT()</t>
-  </si>
-  <si>
-    <t>mod()</t>
-  </si>
-  <si>
     <t>multiplication | Product</t>
   </si>
   <si>
-    <t>count()</t>
-  </si>
-  <si>
-    <t>counta()</t>
-  </si>
-  <si>
     <t>=LEN(A2)</t>
   </si>
   <si>
-    <t>power()</t>
-  </si>
-  <si>
-    <t>sqrt()</t>
-  </si>
-  <si>
     <t>round()</t>
   </si>
   <si>
@@ -551,6 +528,78 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>=PRODUCT(A2:B2)</t>
+  </si>
+  <si>
+    <t>=QUOTIENT(A2,B2)</t>
+  </si>
+  <si>
+    <t>=MOD(A2,B2)</t>
+  </si>
+  <si>
+    <t>=COUNT(A2:B2)</t>
+  </si>
+  <si>
+    <t>dsd</t>
+  </si>
+  <si>
+    <t>gfgf</t>
+  </si>
+  <si>
+    <t>=COUNTA(A2:B2)</t>
+  </si>
+  <si>
+    <t>=POWER(A2,2)</t>
+  </si>
+  <si>
+    <t>=SQRT(A2)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Reference Functions</t>
+  </si>
+  <si>
+    <t>=INDEX(B2:B4, 2)</t>
+  </si>
+  <si>
+    <t>=MATCH("Sarah", A2:A4, 0)</t>
+  </si>
+  <si>
+    <t>=INDIRECT("B2")</t>
+  </si>
+  <si>
+    <t>=OFFSET(B2, 1, 0)</t>
+  </si>
+  <si>
+    <t>=CHOOSE(2, "Red", "Green", "Blue")</t>
+  </si>
+  <si>
+    <t>=ROW(A3)</t>
+  </si>
+  <si>
+    <t>=COLUMN(B2)</t>
+  </si>
+  <si>
+    <t>INDEX(), MATCH(), INDIRECT(), OFFSET(), CHOOSE(), ROW(), COLUMN()</t>
+  </si>
+  <si>
+    <t>sdsfds</t>
   </si>
 </sst>
 </file>
@@ -659,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -697,6 +746,16 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -707,9 +766,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -720,14 +778,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1008,17 +1073,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -1032,49 +1105,49 @@
         <v>126</v>
       </c>
       <c r="D1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" t="s">
+        <v>130</v>
+      </c>
+      <c r="O1" t="s">
+        <v>131</v>
+      </c>
+      <c r="P1" t="s">
         <v>132</v>
       </c>
-      <c r="E1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="J1" t="s">
+      <c r="R1" t="s">
         <v>134</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="L1" t="s">
-        <v>136</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="N1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O1" t="s">
-        <v>139</v>
-      </c>
-      <c r="P1" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="R1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -1085,8 +1158,8 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <f>SUM(A2:B2)</f>
-        <v>333</v>
+        <f>SUM(A2:B2,F12:F13,H12:K12)</f>
+        <v>349</v>
       </c>
       <c r="D2">
         <f>A2*B2</f>
@@ -1101,7 +1174,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G2" t="e">
-        <f t="shared" ref="G2:G12" si="0">MOD(A2,B2)</f>
+        <f t="shared" ref="G2:G13" si="0">MOD(A2,B2)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H2">
@@ -1117,24 +1190,24 @@
         <v>2</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K16" si="2">LEN(A3)</f>
+        <f>LEN(A2)</f>
         <v>3</v>
       </c>
       <c r="L2">
-        <f>POWER(2,2)</f>
-        <v>4</v>
+        <f>POWER(A2,2)</f>
+        <v>110889</v>
       </c>
       <c r="M2">
         <f>SQRT(A2)</f>
         <v>18.248287590894659</v>
       </c>
       <c r="N2">
-        <f>ROUND(M2,2)</f>
-        <v>18.25</v>
+        <f>ROUND(M2,0)</f>
+        <v>18</v>
       </c>
       <c r="O2">
-        <f>CEILING(M2,1)</f>
-        <v>19</v>
+        <f>CEILING(M2,2)</f>
+        <v>20</v>
       </c>
       <c r="P2">
         <f>ROUNDUP(M2,0)</f>
@@ -1142,83 +1215,71 @@
       </c>
       <c r="Q2">
         <f ca="1">RAND()</f>
-        <v>0.78110030991428259</v>
+        <v>2.020854478473566E-2</v>
       </c>
       <c r="R2">
-        <f ca="1">RANDBETWEEN(100,1000)</f>
-        <v>166</v>
+        <f ca="1">RANDBETWEEN(1000,9999)</f>
+        <v>3695</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
-        <v>333</v>
+        <v>11</v>
       </c>
       <c r="B3" s="12">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C6" si="3">SUM(A3:B3)</f>
-        <v>358</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D6" si="4">A3*B3</f>
-        <v>8325</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E15" si="5">PRODUCT(A3:B3)</f>
-        <v>8325</v>
+        <f t="shared" ref="C3:C22" si="2">SUM(A3:B3)</f>
+        <v>13</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F15" si="6">QUOTIENT(A3,B3)</f>
-        <v>13</v>
+        <f t="shared" ref="F3:F7" si="3">QUOTIENT(A3,B3)</f>
+        <v>5</v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" si="1"/>
-        <v>179</v>
+        <v>6.5</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I15" si="7">COUNT(A3:B3)</f>
+        <f t="shared" ref="I3:I11" si="4">COUNT(A3:B3)</f>
         <v>2</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J16" si="8">COUNTA(A3:B3)</f>
+        <f t="shared" ref="J3:J22" si="5">COUNTA(A3:B3)</f>
         <v>2</v>
       </c>
       <c r="K3">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" ref="K3:K22" si="6">LEN(A3)</f>
+        <v>2</v>
       </c>
       <c r="L3">
-        <f>POWER(A3,3)</f>
-        <v>36926037</v>
+        <f>POWER(A3,K2)</f>
+        <v>1331</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M16" si="9">SQRT(A3)</f>
-        <v>18.248287590894659</v>
+        <f t="shared" ref="M3:M26" si="7">SQRT(A3)</f>
+        <v>3.3166247903553998</v>
       </c>
       <c r="N3">
-        <f>ROUND(M3,3)</f>
-        <v>18.248000000000001</v>
-      </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O16" si="10">CEILING(M3,1)</f>
-        <v>19</v>
+        <f t="shared" ref="N3:N26" si="8">ROUND(M3,2)</f>
+        <v>3.32</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P16" si="11">ROUNDUP(M3,0)</f>
-        <v>19</v>
+        <f t="shared" ref="P3:P26" si="9">ROUNDUP(M3,0)</f>
+        <v>4</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q16" ca="1" si="12">RAND()</f>
-        <v>0.94561602312717785</v>
+        <f ca="1">RAND()</f>
+        <v>0.45597828801362417</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R16" ca="1" si="13">RANDBETWEEN(100,1000)</f>
-        <v>559</v>
+        <f t="shared" ref="R3:R26" ca="1" si="10">RANDBETWEEN(1000,9999)</f>
+        <v>1018</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -1229,19 +1290,11 @@
         <v>0</v>
       </c>
       <c r="C4">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+      <c r="F4" t="e">
         <f t="shared" si="3"/>
-        <v>333</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F4" t="e">
-        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="G4" t="e">
@@ -1253,44 +1306,40 @@
         <v>166.5</v>
       </c>
       <c r="I4">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L26" si="11">POWER(A4,K3)</f>
+        <v>110889</v>
+      </c>
+      <c r="M4">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="J4">
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N4">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L16" si="14">POWER(A4,3)</f>
-        <v>36926037</v>
-      </c>
-      <c r="M4">
+        <v>18.25</v>
+      </c>
+      <c r="P4">
         <f t="shared" si="9"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N4">
-        <f t="shared" ref="N4:N16" si="15">ROUND(M4,2)</f>
-        <v>18.25</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="10"/>
         <v>19</v>
       </c>
-      <c r="P4">
-        <f t="shared" si="11"/>
-        <v>19</v>
-      </c>
       <c r="Q4">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.48896558051248562</v>
+        <f ca="1">RAND()</f>
+        <v>0.25352140659950084</v>
       </c>
       <c r="R4">
-        <f t="shared" ca="1" si="13"/>
-        <v>812</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>9964</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1301,19 +1350,11 @@
         <v>45</v>
       </c>
       <c r="C5">
+        <f t="shared" si="2"/>
+        <v>378</v>
+      </c>
+      <c r="F5">
         <f t="shared" si="3"/>
-        <v>378</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="4"/>
-        <v>14985</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="5"/>
-        <v>14985</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="G5">
@@ -1325,44 +1366,40 @@
         <v>189</v>
       </c>
       <c r="I5">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="11"/>
+        <v>36926037</v>
+      </c>
+      <c r="M5">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="J5">
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N5">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="14"/>
-        <v>36926037</v>
-      </c>
-      <c r="M5">
+        <v>18.25</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="9"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N5">
-        <f>ROUND(M5,0)</f>
-        <v>18</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="10"/>
         <v>19</v>
       </c>
-      <c r="P5">
-        <f t="shared" si="11"/>
-        <v>19</v>
-      </c>
       <c r="Q5">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.98660386632513752</v>
+        <f t="shared" ref="Q5:Q26" ca="1" si="12">RAND()</f>
+        <v>0.39742473012675983</v>
       </c>
       <c r="R5">
-        <f t="shared" ca="1" si="13"/>
-        <v>919</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>5055</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -1373,19 +1410,11 @@
         <v>55</v>
       </c>
       <c r="C6">
+        <f t="shared" si="2"/>
+        <v>388</v>
+      </c>
+      <c r="F6">
         <f t="shared" si="3"/>
-        <v>388</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="4"/>
-        <v>18315</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="5"/>
-        <v>18315</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="G6">
@@ -1397,691 +1426,963 @@
         <v>194</v>
       </c>
       <c r="I6">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="11"/>
+        <v>36926037</v>
+      </c>
+      <c r="M6">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="J6">
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N6">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="14"/>
-        <v>36926037</v>
-      </c>
-      <c r="M6">
+        <v>18.25</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="9"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="15"/>
-        <v>18.25</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="10"/>
-        <v>19</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="12"/>
-        <v>0.80457349761848052</v>
+        <v>3.6166457913349159E-2</v>
       </c>
       <c r="R6">
-        <f t="shared" ca="1" si="13"/>
-        <v>208</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>2749</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>3333</v>
-      </c>
-      <c r="B7">
-        <f>SUM(B2:B6)</f>
-        <v>125</v>
+      <c r="A7" s="12">
+        <v>333</v>
+      </c>
+      <c r="B7" s="12">
+        <v>65</v>
       </c>
       <c r="C7">
-        <f>SUM(C2:C6)</f>
-        <v>1790</v>
-      </c>
-      <c r="D7">
-        <f>SUM(D2:D6)</f>
-        <v>41625</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="5"/>
-        <v>416625</v>
+        <f t="shared" si="2"/>
+        <v>398</v>
       </c>
       <c r="F7">
-        <f t="shared" si="6"/>
-        <v>26</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>1729</v>
+        <v>199</v>
       </c>
       <c r="I7">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="11"/>
+        <v>36926037</v>
+      </c>
+      <c r="M7">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="J7">
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N7">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="14"/>
-        <v>37025927037</v>
-      </c>
-      <c r="M7">
+        <v>18.25</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="9"/>
-        <v>57.732140095444237</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="15"/>
-        <v>57.73</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="10"/>
-        <v>58</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="11"/>
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="12"/>
-        <v>0.76339599531035929</v>
+        <v>0.17102530386929771</v>
       </c>
       <c r="R7">
-        <f t="shared" ca="1" si="13"/>
-        <v>979</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>3392</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <f>AVERAGE(A2:A7)</f>
-        <v>833</v>
-      </c>
-      <c r="B8">
-        <f>AVERAGE(B2:B7)</f>
-        <v>41.666666666666664</v>
+      <c r="A8" s="12">
+        <v>333</v>
+      </c>
+      <c r="B8" s="12">
+        <v>75</v>
       </c>
       <c r="C8">
-        <f>AVERAGE(C2:C7)</f>
-        <v>596.66666666666663</v>
-      </c>
-      <c r="D8">
-        <f>AVERAGE(D2:D7)</f>
-        <v>13875</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="5"/>
-        <v>34708.333333333328</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="6"/>
-        <v>19</v>
+        <f t="shared" si="2"/>
+        <v>408</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>41.333333333333378</v>
+        <v>33</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>437.33333333333331</v>
+        <v>204</v>
       </c>
       <c r="I8">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="11"/>
+        <v>36926037</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="J8">
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N8">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="14"/>
-        <v>578009537</v>
-      </c>
-      <c r="M8">
+        <v>18.25</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="9"/>
-        <v>28.861739379323623</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="15"/>
-        <v>28.86</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="10"/>
-        <v>29</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="11"/>
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="12"/>
-        <v>0.16880788051704509</v>
+        <v>0.43907719544375279</v>
       </c>
       <c r="R8">
-        <f t="shared" ca="1" si="13"/>
-        <v>122</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>8218</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <f>MAX(A2:A8)</f>
-        <v>3333</v>
-      </c>
-      <c r="B9">
-        <f>MAX(B2:B8)</f>
-        <v>125</v>
+      <c r="A9" s="12">
+        <v>333</v>
+      </c>
+      <c r="B9" s="12">
+        <v>85</v>
       </c>
       <c r="C9">
-        <f>MAX(C2:C8)</f>
-        <v>1790</v>
-      </c>
-      <c r="D9">
-        <f>MAX(D2:D8)</f>
-        <v>41625</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="5"/>
-        <v>416625</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="6"/>
-        <v>26</v>
+        <f t="shared" si="2"/>
+        <v>418</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="H9">
         <f t="shared" si="1"/>
-        <v>1729</v>
+        <v>209</v>
       </c>
       <c r="I9">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="11"/>
+        <v>36926037</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="J9">
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N9">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="2"/>
-        <v>3</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="14"/>
-        <v>37025927037</v>
-      </c>
-      <c r="M9">
+        <v>18.25</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="9"/>
-        <v>57.732140095444237</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="15"/>
-        <v>57.73</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="10"/>
-        <v>58</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="11"/>
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="12"/>
-        <v>0.73204195694662977</v>
+        <v>0.92290173882400794</v>
       </c>
       <c r="R9">
-        <f t="shared" ca="1" si="13"/>
-        <v>353</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>3436</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <f>MIN(A2:A9)</f>
-        <v>333</v>
-      </c>
-      <c r="B10">
-        <f>MIN(B2:B9)</f>
-        <v>0</v>
+      <c r="A10" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="12">
+        <v>95</v>
       </c>
       <c r="C10">
-        <f>MIN(C2:C9)</f>
-        <v>333</v>
-      </c>
-      <c r="D10">
-        <f>MIN(D2:D9)</f>
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F10" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
+        <f t="shared" si="2"/>
+        <v>95</v>
       </c>
       <c r="G10" t="e">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>#VALUE!</v>
       </c>
       <c r="H10">
         <f t="shared" si="1"/>
-        <v>166.5</v>
+        <v>95</v>
       </c>
       <c r="I10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="L10" t="e">
+        <f t="shared" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M10" t="e">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="J10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N10" t="e">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="14"/>
-        <v>36926037</v>
-      </c>
-      <c r="M10">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P10" t="e">
         <f t="shared" si="9"/>
-        <v>18.248287590894659</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="15"/>
-        <v>18.25</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="10"/>
-        <v>19</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="11"/>
-        <v>19</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="12"/>
-        <v>0.8522242868489639</v>
+        <v>0.10346744407497654</v>
       </c>
       <c r="R10">
-        <f t="shared" ca="1" si="13"/>
-        <v>570</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>5334</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f>COUNT(A2:A10)</f>
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <f>COUNT(B2:B10)</f>
-        <v>9</v>
+      <c r="A11" s="12">
+        <v>333</v>
+      </c>
+      <c r="B11" s="12">
+        <v>105</v>
       </c>
       <c r="C11">
-        <f>COUNT(C2:C10)</f>
-        <v>9</v>
-      </c>
-      <c r="D11">
-        <f>COUNT(D2:D10)</f>
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="5"/>
-        <v>81</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="6"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>438</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="H11">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>219</v>
       </c>
       <c r="I11">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="11"/>
+        <v>12296370321</v>
+      </c>
+      <c r="M11">
         <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="J11">
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N11">
         <f t="shared" si="8"/>
-        <v>2</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <f t="shared" si="14"/>
-        <v>729</v>
-      </c>
-      <c r="M11">
+        <v>18.25</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="9"/>
-        <v>3</v>
-      </c>
-      <c r="N11">
-        <f t="shared" si="15"/>
-        <v>3</v>
-      </c>
-      <c r="O11">
-        <f t="shared" si="10"/>
-        <v>3</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="11"/>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="12"/>
-        <v>0.68442828288013036</v>
+        <v>0.20465925443815247</v>
       </c>
       <c r="R11">
-        <f t="shared" ca="1" si="13"/>
-        <v>968</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>6691</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E12">
+      <c r="A12" s="12">
+        <v>22</v>
+      </c>
+      <c r="B12" s="12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="11"/>
+        <v>10648</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="7"/>
+        <v>4.6904157598234297</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="8"/>
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.5351918660958993</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ca="1" si="10"/>
+        <v>3775</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>22</v>
+      </c>
+      <c r="B13" s="12">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="11"/>
+        <v>484</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="7"/>
+        <v>4.6904157598234297</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="8"/>
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.11141073604076834</v>
+      </c>
+      <c r="R13">
+        <f t="shared" ca="1" si="10"/>
+        <v>2147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>22</v>
+      </c>
+      <c r="B14" s="12">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="11"/>
+        <v>484</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="7"/>
+        <v>4.6904157598234297</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="8"/>
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.62777605526711044</v>
+      </c>
+      <c r="R14">
+        <f t="shared" ca="1" si="10"/>
+        <v>7699</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>22</v>
+      </c>
+      <c r="B15" s="12">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="11"/>
+        <v>484</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="7"/>
+        <v>4.6904157598234297</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="8"/>
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.36845397457125595</v>
+      </c>
+      <c r="R15">
+        <f t="shared" ca="1" si="10"/>
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="12">
+        <v>22</v>
+      </c>
+      <c r="B16" s="12">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="11"/>
+        <v>484</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="7"/>
+        <v>4.6904157598234297</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="8"/>
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.27917360944603842</v>
+      </c>
+      <c r="R16">
+        <f t="shared" ca="1" si="10"/>
+        <v>7104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="12">
+        <v>22</v>
+      </c>
+      <c r="B17" s="12">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="11"/>
+        <v>484</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="7"/>
+        <v>4.6904157598234297</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="8"/>
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.91898222875859792</v>
+      </c>
+      <c r="R17">
+        <f t="shared" ca="1" si="10"/>
+        <v>4763</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="12">
+        <v>22</v>
+      </c>
+      <c r="B18" s="12">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="11"/>
+        <v>484</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="7"/>
+        <v>4.6904157598234297</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="8"/>
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.80711590906124986</v>
+      </c>
+      <c r="R18">
+        <f t="shared" ca="1" si="10"/>
+        <v>6993</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f>SUM(A2:A18)</f>
+        <v>2829</v>
+      </c>
+      <c r="B19">
+        <f>SUM(B2:B18)</f>
+        <v>611</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="2"/>
+        <v>3440</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="11"/>
+        <v>8003241</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="7"/>
+        <v>53.1883445878888</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="8"/>
+        <v>53.19</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="9"/>
+        <v>54</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.17498299287542829</v>
+      </c>
+      <c r="R19">
+        <f t="shared" ca="1" si="10"/>
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f>AVERAGE(A2:A18)</f>
+        <v>176.8125</v>
+      </c>
+      <c r="B20">
+        <f>AVERAGE(B2:B18)</f>
+        <v>35.941176470588232</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>212.75367647058823</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="11"/>
+        <v>977353920.04518127</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="7"/>
+        <v>13.2970861469722</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="8"/>
+        <v>13.3</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="9"/>
+        <v>14</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.43310641016835982</v>
+      </c>
+      <c r="R20">
+        <f t="shared" ca="1" si="10"/>
+        <v>6171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f>COUNT(A2:A18)</f>
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <f>COUNT(B2:B18)</f>
+        <v>17</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="11"/>
+        <v>4294967296</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="N21">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.86380326826751141</v>
+      </c>
+      <c r="R21">
+        <f t="shared" ca="1" si="10"/>
+        <v>7619</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f>MAX(A2:A18)</f>
+        <v>333</v>
+      </c>
+      <c r="B22">
+        <f>MAX(B2:B18)</f>
+        <v>105</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>438</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="11"/>
+        <v>110889</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="7"/>
+        <v>18.248287590894659</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="8"/>
+        <v>18.25</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="9"/>
+        <v>19</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.26540491412597089</v>
+      </c>
+      <c r="R22">
+        <f t="shared" ca="1" si="10"/>
+        <v>2573</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f>MIN(A2:A18)</f>
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <f>MIN(B2:B18)</f>
         <v>0</v>
       </c>
-      <c r="F12" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G12" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H12">
-        <v>33</v>
-      </c>
-      <c r="I12">
+      <c r="L23">
+        <f t="shared" si="11"/>
+        <v>1331</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="7"/>
+        <v>3.3166247903553998</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="8"/>
+        <v>3.32</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.3488310700022843</v>
+      </c>
+      <c r="R23">
+        <f t="shared" ca="1" si="10"/>
+        <v>9384</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <f>COUNT(A2:A18,A25:A26)</f>
+        <v>16</v>
+      </c>
+      <c r="L24" t="e">
+        <f t="shared" si="11"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="M24">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="J12">
+      <c r="N24">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="K12">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="M12">
+      <c r="P24">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="N12">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P12">
+      <c r="Q24">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.16303416914360946</v>
+      </c>
+      <c r="R24">
+        <f t="shared" ca="1" si="10"/>
+        <v>5968</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>170</v>
+      </c>
+      <c r="F25">
+        <f>COUNTA(A2:A18,A25:A26)</f>
+        <v>19</v>
+      </c>
+      <c r="L25" t="e">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.66244324087640438</v>
-      </c>
-      <c r="R12">
-        <f t="shared" ca="1" si="13"/>
-        <v>666</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>127</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F13" t="e">
-        <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="G13">
-        <v>33</v>
-      </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
-      <c r="I13">
+      <c r="M25" t="e">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J13">
-        <f>COUNTA(A13:B13)</f>
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="L13" t="e">
-        <f t="shared" si="14"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M13" t="e">
+      <c r="N25" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P25" t="e">
         <f t="shared" si="9"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N13" t="e">
-        <f t="shared" si="15"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O13" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P13" t="e">
+      <c r="Q25">
+        <f t="shared" ca="1" si="12"/>
+        <v>0.85232339580307004</v>
+      </c>
+      <c r="R25">
+        <f t="shared" ca="1" si="10"/>
+        <v>9803</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>170</v>
+      </c>
+      <c r="L26" t="e">
         <f t="shared" si="11"/>
         <v>#VALUE!</v>
       </c>
-      <c r="Q13">
+      <c r="M26" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N26" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P26" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q26">
         <f t="shared" ca="1" si="12"/>
-        <v>0.91636972576779496</v>
-      </c>
-      <c r="R13">
-        <f t="shared" ca="1" si="13"/>
-        <v>674</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="5"/>
-        <v>2</v>
-      </c>
-      <c r="F14" t="e">
-        <f>QUOTIENT(A14,B14)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14">
-        <v>33</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="14"/>
-        <v>8</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="9"/>
-        <v>1.4142135623730951</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="15"/>
-        <v>1.41</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="11"/>
-        <v>2</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.80965757593807008</v>
-      </c>
-      <c r="R14">
-        <f t="shared" ca="1" si="13"/>
-        <v>768</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E15">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="F15" t="e">
-        <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15">
-        <v>33</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.9841513342958369</v>
-      </c>
-      <c r="R15">
-        <f t="shared" ca="1" si="13"/>
-        <v>614</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="E16">
-        <f>PRODUCT(A16:B16)</f>
-        <v>0</v>
-      </c>
-      <c r="F16" t="e">
-        <f>QUOTIENT(A16,B16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H16">
-        <v>33</v>
-      </c>
-      <c r="I16">
-        <f>COUNT(A16:B16)</f>
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="O16">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" ca="1" si="12"/>
-        <v>0.82182337475158085</v>
-      </c>
-      <c r="R16">
-        <f t="shared" ca="1" si="13"/>
-        <v>714</v>
+        <v>0.7988890497600476</v>
+      </c>
+      <c r="R26">
+        <f t="shared" ca="1" si="10"/>
+        <v>3463</v>
       </c>
     </row>
   </sheetData>
@@ -2124,57 +2425,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
     </row>
     <row r="2" spans="1:29" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -2245,7 +2546,7 @@
         <v>69</v>
       </c>
       <c r="T3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="U3" t="s">
         <v>70</v>
@@ -2300,7 +2601,7 @@
       </c>
       <c r="L4" t="str">
         <f ca="1">TEXT(TODAY(),"mm/dd/yyyy")</f>
-        <v>02/10/2025</v>
+        <v>02/13/2025</v>
       </c>
       <c r="M4" t="str">
         <f>LEFT(F4,5)</f>
@@ -2340,7 +2641,7 @@
       </c>
       <c r="W4" t="str">
         <f ca="1">SUBSTITUTE(L4,"/","-")</f>
-        <v>02-10-2025</v>
+        <v>02-13-2025</v>
       </c>
       <c r="X4">
         <f>FIND("Trichy",K4)</f>
@@ -2484,7 +2785,7 @@
       </c>
       <c r="L7" s="3">
         <f ca="1">TODAY()</f>
-        <v>45698</v>
+        <v>45701</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
@@ -3579,13 +3880,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="29" t="s">
         <v>87</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -3632,9 +3933,9 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
       <c r="D2" s="7" t="s">
         <v>99</v>
       </c>
@@ -3679,9 +3980,9 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="9" t="s">
         <v>110</v>
       </c>
@@ -4103,382 +4404,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C5" s="3">
-        <f>DATE(2020,12,10)</f>
-        <v>44175</v>
-      </c>
-      <c r="D5" s="3">
-        <f ca="1">TODAY()</f>
-        <v>45698</v>
-      </c>
-      <c r="E5" s="4">
-        <f ca="1">NOW()</f>
-        <v>45698.635017592591</v>
-      </c>
-      <c r="F5" s="5">
-        <f>TIME(2,30,30)</f>
-        <v>0.10451388888888889</v>
-      </c>
-      <c r="G5">
-        <f ca="1">DATEDIF(C5,D5,"ym")</f>
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <f ca="1">YEAR(D5)</f>
-        <v>2025</v>
-      </c>
-      <c r="I5">
-        <f ca="1">DAY(D5)</f>
-        <v>10</v>
-      </c>
-      <c r="J5">
-        <f ca="1">HOUR(E5)</f>
-        <v>15</v>
-      </c>
-      <c r="K5">
-        <f ca="1">MINUTE(E5)</f>
-        <v>14</v>
-      </c>
-      <c r="L5">
-        <f ca="1">SECOND(E5)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I9" s="20">
-        <v>12</v>
-      </c>
-      <c r="J9">
-        <v>12</v>
-      </c>
-      <c r="K9">
-        <v>2002</v>
-      </c>
-      <c r="L9" s="3">
-        <f>DATE(K9,J9,I9)</f>
-        <v>37602</v>
-      </c>
-      <c r="N9" s="3">
-        <v>37602</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="D10" s="3">
-        <f ca="1">TODAY()</f>
-        <v>45698</v>
-      </c>
-      <c r="E10">
-        <f ca="1">YEAR(D10)</f>
-        <v>2025</v>
-      </c>
-      <c r="F10">
-        <f ca="1">MONTH(E10)</f>
-        <v>7</v>
-      </c>
-      <c r="G10">
-        <f ca="1">YEARFRAC(TODAY(),C5)</f>
-        <v>4.166666666666667</v>
-      </c>
-      <c r="I10" s="20">
-        <v>12</v>
-      </c>
-      <c r="J10">
-        <v>12</v>
-      </c>
-      <c r="K10">
-        <v>2001</v>
-      </c>
-      <c r="L10" s="3">
-        <f t="shared" ref="L10:L18" si="0">DATE(K10,J10,I10)</f>
-        <v>37237</v>
-      </c>
-      <c r="N10" s="3">
-        <v>37237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="D11" s="4">
-        <f ca="1">NOW()</f>
-        <v>45698.635017592591</v>
-      </c>
-      <c r="I11" s="20">
-        <v>12</v>
-      </c>
-      <c r="J11">
-        <v>12</v>
-      </c>
-      <c r="K11">
-        <v>2001</v>
-      </c>
-      <c r="L11" s="3">
-        <f t="shared" si="0"/>
-        <v>37237</v>
-      </c>
-      <c r="M11">
-        <f>DATEDIF(L11,L13,"Y")</f>
-        <v>800</v>
-      </c>
-      <c r="N11" s="3">
-        <v>37237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I12" s="20"/>
-      <c r="L12" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N12" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E13" s="19">
-        <v>0.61597222222222225</v>
-      </c>
-      <c r="G13" s="4">
-        <v>45695.616666666669</v>
-      </c>
-      <c r="I13" s="20">
-        <v>12</v>
-      </c>
-      <c r="J13">
-        <v>12</v>
-      </c>
-      <c r="K13">
-        <v>2801</v>
-      </c>
-      <c r="L13" s="3">
-        <f>DATE(K13,J13,I13)</f>
-        <v>329431</v>
-      </c>
-      <c r="N13" s="3">
-        <v>329431</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E14" s="3">
-        <f ca="1">TODAY()</f>
-        <v>45698</v>
-      </c>
-      <c r="I14" s="20"/>
-      <c r="L14" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N14" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E15" s="3">
-        <v>45695</v>
-      </c>
-      <c r="G15" s="4">
-        <f ca="1">NOW()</f>
-        <v>45698.635017592591</v>
-      </c>
-      <c r="I15" s="20">
-        <v>12</v>
-      </c>
-      <c r="J15">
-        <v>12</v>
-      </c>
-      <c r="K15">
-        <v>2009</v>
-      </c>
-      <c r="L15" s="3">
-        <f>DATE(K15,J15,I15)</f>
-        <v>40159</v>
-      </c>
-      <c r="N15" s="3">
-        <v>40159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E16" s="19">
-        <v>0.61597222222222225</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="L16" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N16" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="I17" s="20"/>
-      <c r="L17" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N17" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E18" s="3">
-        <v>45695</v>
-      </c>
-      <c r="I18" s="20">
-        <v>12</v>
-      </c>
-      <c r="J18">
-        <v>12</v>
-      </c>
-      <c r="K18">
-        <v>2001</v>
-      </c>
-      <c r="L18" s="3">
-        <f t="shared" si="0"/>
-        <v>37237</v>
-      </c>
-      <c r="N18" s="3">
-        <v>37237</v>
-      </c>
-    </row>
-    <row r="19" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E19" s="19">
-        <v>0.61597222222222225</v>
-      </c>
-      <c r="L19" t="s">
-        <v>144</v>
-      </c>
-      <c r="N19" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E20" s="19">
-        <v>0.6166666666666667</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="G2:N2"/>
-    <mergeCell ref="A1:T1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" customWidth="1"/>
-    <col min="10" max="10" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
-        <v>146</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -4499,22 +4426,23 @@
       <c r="R1" s="28"/>
       <c r="S1" s="28"/>
       <c r="T1" s="28"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="27" t="s">
+        <v>59</v>
+      </c>
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
@@ -4522,66 +4450,439 @@
       <c r="L2" s="27"/>
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C5" s="3">
+        <f>DATE(2020,12,10)</f>
+        <v>44175</v>
+      </c>
+      <c r="D5" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45701</v>
+      </c>
+      <c r="E5" s="4">
+        <f ca="1">NOW()</f>
+        <v>45701.494058564815</v>
+      </c>
+      <c r="F5" s="5">
+        <f>TIME(2,30,30)</f>
+        <v>0.10451388888888889</v>
+      </c>
+      <c r="G5">
+        <f ca="1">DATEDIF(C5,D5,"ym")</f>
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f ca="1">YEAR(D5)</f>
+        <v>2025</v>
+      </c>
+      <c r="I5">
+        <f ca="1">DAY(D5)</f>
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <f ca="1">HOUR(E5)</f>
+        <v>11</v>
+      </c>
+      <c r="K5">
+        <f ca="1">MINUTE(E5)</f>
+        <v>51</v>
+      </c>
+      <c r="L5">
+        <f ca="1">SECOND(E5)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I9" s="20">
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+      <c r="K9">
+        <v>2002</v>
+      </c>
+      <c r="L9" s="3">
+        <f>DATE(K9,J9,I9)</f>
+        <v>37602</v>
+      </c>
+      <c r="N9" s="3">
+        <v>37602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D10" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45701</v>
+      </c>
+      <c r="E10">
+        <f ca="1">YEAR(D10)</f>
+        <v>2025</v>
+      </c>
+      <c r="F10">
+        <f ca="1">MONTH(E10)</f>
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <f ca="1">YEARFRAC(TODAY(),C5)</f>
+        <v>4.1749999999999998</v>
+      </c>
+      <c r="I10" s="20">
+        <v>12</v>
+      </c>
+      <c r="J10">
+        <v>12</v>
+      </c>
+      <c r="K10">
+        <v>2001</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" ref="L10:L18" si="0">DATE(K10,J10,I10)</f>
+        <v>37237</v>
+      </c>
+      <c r="N10" s="3">
+        <v>37237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D11" s="4">
+        <f ca="1">NOW()</f>
+        <v>45701.494058564815</v>
+      </c>
+      <c r="I11" s="20">
+        <v>12</v>
+      </c>
+      <c r="J11">
+        <v>12</v>
+      </c>
+      <c r="K11">
+        <v>2001</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="0"/>
+        <v>37237</v>
+      </c>
+      <c r="M11">
+        <f>DATEDIF(L11,L13,"Y")</f>
+        <v>800</v>
+      </c>
+      <c r="N11" s="3">
+        <v>37237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I12" s="20"/>
+      <c r="L12" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N12" s="3" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="E13" s="19">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="G13" s="4">
+        <v>45695.616666666669</v>
+      </c>
+      <c r="I13" s="20">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>2801</v>
+      </c>
+      <c r="L13" s="3">
+        <f>DATE(K13,J13,I13)</f>
+        <v>329431</v>
+      </c>
+      <c r="N13" s="3">
+        <v>329431</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="E14" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45701</v>
+      </c>
+      <c r="I14" s="20"/>
+      <c r="L14" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N14" s="3" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="E15" s="3">
+        <v>45695</v>
+      </c>
+      <c r="G15" s="4">
+        <f ca="1">NOW()</f>
+        <v>45701.494058564815</v>
+      </c>
+      <c r="I15" s="20">
+        <v>12</v>
+      </c>
+      <c r="J15">
+        <v>12</v>
+      </c>
+      <c r="K15">
+        <v>2009</v>
+      </c>
+      <c r="L15" s="3">
+        <f>DATE(K15,J15,I15)</f>
+        <v>40159</v>
+      </c>
+      <c r="N15" s="3">
+        <v>40159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="E16" s="19">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="I16" s="20"/>
+      <c r="L16" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N16" s="3" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="I17" s="20"/>
+      <c r="L17" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N17" s="3" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E18" s="3">
+        <v>45695</v>
+      </c>
+      <c r="I18" s="20">
+        <v>12</v>
+      </c>
+      <c r="J18">
+        <v>12</v>
+      </c>
+      <c r="K18">
+        <v>2001</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" si="0"/>
+        <v>37237</v>
+      </c>
+      <c r="N18" s="3">
+        <v>37237</v>
+      </c>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E19" s="19">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="L19" t="s">
+        <v>136</v>
+      </c>
+      <c r="N19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E20" s="19">
+        <v>0.6166666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G2:N2"/>
+    <mergeCell ref="A1:T1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" customWidth="1"/>
+    <col min="10" max="10" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="30" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="E4" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="F4" s="30" t="s">
+      <c r="J4" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="G4" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="H4" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="J4" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="K4" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="L4" s="30" t="s">
-        <v>161</v>
-      </c>
-      <c r="M4" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="N4" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
+      <c r="K4" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="M4" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
@@ -4629,7 +4930,7 @@
         <f>MIN(B5:B9)</f>
         <v>0</v>
       </c>
-      <c r="M5" s="24">
+      <c r="M5" s="21">
         <f>STDEV(A5:A9)</f>
         <v>7.6681158050723228</v>
       </c>
@@ -4734,16 +5035,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N11">
+        <f>SQRT(N5)</f>
+        <v>7.6681158050723228</v>
+      </c>
+    </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H15" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="29"/>
+      <c r="A16" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="30"/>
       <c r="C16">
         <v>1</v>
       </c>
@@ -4765,10 +5072,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="B17" s="29"/>
+      <c r="A17" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="30"/>
       <c r="C17">
         <v>1</v>
       </c>
@@ -4788,7 +5095,7 @@
         <v>3</v>
       </c>
       <c r="I17" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -4810,8 +5117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4822,70 +5129,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B1" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
+      <c r="B1" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="D2" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
+      <c r="C2" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -4912,21 +5219,21 @@
         <v>55</v>
       </c>
       <c r="C6" s="12">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>170</v>
+      <c r="G6" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" s="25" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B7" s="12">
         <v>30</v>
@@ -4937,17 +5244,17 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="31" t="s">
+      <c r="G7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="31">
-        <f>VLOOKUP(G7,A5:F26,2)</f>
-        <v>40</v>
+      <c r="H7" s="24">
+        <f>VLOOKUP(G7,A5:F9,3)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B8" s="12">
         <v>40</v>
@@ -4956,7 +5263,7 @@
         <v>45</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E8" s="12">
         <v>33</v>
@@ -4964,17 +5271,17 @@
       <c r="F8" s="12">
         <v>333</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="31">
-        <f>VLOOKUP(G8,A5:F26,3)</f>
-        <v>25</v>
+      <c r="H8" s="24">
+        <f>VLOOKUP(G8,A5:F9,3)</f>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B9" s="12">
         <v>50</v>
@@ -4985,10 +5292,17 @@
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
+      <c r="G9" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="H9" s="24">
+        <f>VLOOKUP(G9,A5:F9,3)</f>
+        <v>55</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H15" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
@@ -5002,19 +5316,19 @@
         <v>34</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="H16" s="33" t="s">
-        <v>171</v>
+        <v>158</v>
+      </c>
+      <c r="G16" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="H16" s="26" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -5036,17 +5350,17 @@
       <c r="F17" s="12">
         <v>50</v>
       </c>
-      <c r="G17" s="31" t="s">
-        <v>173</v>
-      </c>
-      <c r="H17" s="32">
+      <c r="G17" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="H17" s="25">
         <f>HLOOKUP(G17,A16:F26,2,)</f>
         <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B18" s="12">
         <v>0</v>
@@ -5063,10 +5377,10 @@
       <c r="F18" s="12">
         <v>55</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="24">
         <v>50</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="25">
         <f>HLOOKUP(G18,B17:F21,2,TRUE)</f>
         <v>55</v>
       </c>
@@ -5076,7 +5390,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="12" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F19" s="12"/>
     </row>
@@ -5108,4 +5422,227 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" s="35" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D2" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
+      <c r="S3" s="38"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" s="39">
+        <v>25</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="38">
+        <f>INDEX(A4:B7, 3,2)</f>
+        <v>30</v>
+      </c>
+      <c r="E5" s="38">
+        <f>MATCH("Sarah", A4:A7, 0)</f>
+        <v>3</v>
+      </c>
+      <c r="F5" s="38">
+        <f ca="1">INDIRECT("B5")</f>
+        <v>25</v>
+      </c>
+      <c r="G5" s="38" t="str">
+        <f ca="1">OFFSET(B5, 2, 1)</f>
+        <v>sdsfds</v>
+      </c>
+      <c r="H5" s="38" t="str">
+        <f>CHOOSE(2, A5,A6,A7)</f>
+        <v>Sarah</v>
+      </c>
+      <c r="I5" s="38">
+        <f>ROW(C7)</f>
+        <v>7</v>
+      </c>
+      <c r="J5" s="38">
+        <f>COLUMN(C7)</f>
+        <v>3</v>
+      </c>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="39" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="39">
+        <v>30</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38">
+        <f>B5</f>
+        <v>25</v>
+      </c>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="38"/>
+      <c r="R6" s="38"/>
+      <c r="S6" s="38"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="B7" s="34">
+        <v>35</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:S1"/>
+    <mergeCell ref="D2:P2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated with logic to solve the taks
</commit_message>
<xml_diff>
--- a/batch_03/Basic_formulas.xlsx
+++ b/batch_03/Basic_formulas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8832" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="8832" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Math Formulas" sheetId="4" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Statistical Functions" sheetId="5" r:id="rId5"/>
     <sheet name="Lookup (V and H _Lookup) " sheetId="6" r:id="rId6"/>
     <sheet name="Reference Functions" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -599,7 +600,7 @@
     <t>INDEX(), MATCH(), INDIRECT(), OFFSET(), CHOOSE(), ROW(), COLUMN()</t>
   </si>
   <si>
-    <t>sdsfds</t>
+    <t>male</t>
   </si>
 </sst>
 </file>
@@ -756,6 +757,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -777,21 +791,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1215,11 +1216,11 @@
       </c>
       <c r="Q2">
         <f ca="1">RAND()</f>
-        <v>2.020854478473566E-2</v>
+        <v>0.19238299205424803</v>
       </c>
       <c r="R2">
         <f ca="1">RANDBETWEEN(1000,9999)</f>
-        <v>3695</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
@@ -1275,11 +1276,11 @@
       </c>
       <c r="Q3">
         <f ca="1">RAND()</f>
-        <v>0.45597828801362417</v>
+        <v>8.62429937706225E-2</v>
       </c>
       <c r="R3">
         <f t="shared" ref="R3:R26" ca="1" si="10">RANDBETWEEN(1000,9999)</f>
-        <v>1018</v>
+        <v>5019</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
@@ -1335,11 +1336,11 @@
       </c>
       <c r="Q4">
         <f ca="1">RAND()</f>
-        <v>0.25352140659950084</v>
+        <v>0.37549659708205807</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="10"/>
-        <v>9964</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
@@ -1395,11 +1396,11 @@
       </c>
       <c r="Q5">
         <f t="shared" ref="Q5:Q26" ca="1" si="12">RAND()</f>
-        <v>0.39742473012675983</v>
+        <v>0.901382427733458</v>
       </c>
       <c r="R5">
         <f t="shared" ca="1" si="10"/>
-        <v>5055</v>
+        <v>6527</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
@@ -1455,11 +1456,11 @@
       </c>
       <c r="Q6">
         <f t="shared" ca="1" si="12"/>
-        <v>3.6166457913349159E-2</v>
+        <v>0.59337110472544152</v>
       </c>
       <c r="R6">
         <f t="shared" ca="1" si="10"/>
-        <v>2749</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
@@ -1515,11 +1516,11 @@
       </c>
       <c r="Q7">
         <f t="shared" ca="1" si="12"/>
-        <v>0.17102530386929771</v>
+        <v>0.29015277845392962</v>
       </c>
       <c r="R7">
         <f t="shared" ca="1" si="10"/>
-        <v>3392</v>
+        <v>2719</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -1571,11 +1572,11 @@
       </c>
       <c r="Q8">
         <f t="shared" ca="1" si="12"/>
-        <v>0.43907719544375279</v>
+        <v>1.2095115990674921E-2</v>
       </c>
       <c r="R8">
         <f t="shared" ca="1" si="10"/>
-        <v>8218</v>
+        <v>2896</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -1627,11 +1628,11 @@
       </c>
       <c r="Q9">
         <f t="shared" ca="1" si="12"/>
-        <v>0.92290173882400794</v>
+        <v>0.57095971936851053</v>
       </c>
       <c r="R9">
         <f t="shared" ca="1" si="10"/>
-        <v>3436</v>
+        <v>5866</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -1683,11 +1684,11 @@
       </c>
       <c r="Q10">
         <f t="shared" ca="1" si="12"/>
-        <v>0.10346744407497654</v>
+        <v>0.75878012035016884</v>
       </c>
       <c r="R10">
         <f t="shared" ca="1" si="10"/>
-        <v>5334</v>
+        <v>7098</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -1739,11 +1740,11 @@
       </c>
       <c r="Q11">
         <f t="shared" ca="1" si="12"/>
-        <v>0.20465925443815247</v>
+        <v>0.84222117507418748</v>
       </c>
       <c r="R11">
         <f t="shared" ca="1" si="10"/>
-        <v>6691</v>
+        <v>2694</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -1797,11 +1798,11 @@
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="12"/>
-        <v>0.5351918660958993</v>
+        <v>6.8908834563663479E-3</v>
       </c>
       <c r="R12">
         <f t="shared" ca="1" si="10"/>
-        <v>3775</v>
+        <v>2332</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -1848,11 +1849,11 @@
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="12"/>
-        <v>0.11141073604076834</v>
+        <v>0.52300600087979587</v>
       </c>
       <c r="R13">
         <f t="shared" ca="1" si="10"/>
-        <v>2147</v>
+        <v>8279</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -1892,11 +1893,11 @@
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="12"/>
-        <v>0.62777605526711044</v>
+        <v>0.1262211183388362</v>
       </c>
       <c r="R14">
         <f t="shared" ca="1" si="10"/>
-        <v>7699</v>
+        <v>5579</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
@@ -1936,11 +1937,11 @@
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="12"/>
-        <v>0.36845397457125595</v>
+        <v>0.49549278636070104</v>
       </c>
       <c r="R15">
         <f t="shared" ca="1" si="10"/>
-        <v>1906</v>
+        <v>5485</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1980,11 +1981,11 @@
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="12"/>
-        <v>0.27917360944603842</v>
+        <v>3.1476734788810856E-2</v>
       </c>
       <c r="R16">
         <f t="shared" ca="1" si="10"/>
-        <v>7104</v>
+        <v>4902</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
@@ -2024,11 +2025,11 @@
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="12"/>
-        <v>0.91898222875859792</v>
+        <v>0.21894267995436323</v>
       </c>
       <c r="R17">
         <f t="shared" ca="1" si="10"/>
-        <v>4763</v>
+        <v>6755</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
@@ -2068,11 +2069,11 @@
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="12"/>
-        <v>0.80711590906124986</v>
+        <v>0.14835729027389588</v>
       </c>
       <c r="R18">
         <f t="shared" ca="1" si="10"/>
-        <v>6993</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
@@ -2114,11 +2115,11 @@
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="12"/>
-        <v>0.17498299287542829</v>
+        <v>8.4073738501228568E-2</v>
       </c>
       <c r="R19">
         <f t="shared" ca="1" si="10"/>
-        <v>2108</v>
+        <v>8138</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
@@ -2160,11 +2161,11 @@
       </c>
       <c r="Q20">
         <f t="shared" ca="1" si="12"/>
-        <v>0.43310641016835982</v>
+        <v>0.7841223982581178</v>
       </c>
       <c r="R20">
         <f t="shared" ca="1" si="10"/>
-        <v>6171</v>
+        <v>5808</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -2206,11 +2207,11 @@
       </c>
       <c r="Q21">
         <f t="shared" ca="1" si="12"/>
-        <v>0.86380326826751141</v>
+        <v>0.77453556935757928</v>
       </c>
       <c r="R21">
         <f t="shared" ca="1" si="10"/>
-        <v>7619</v>
+        <v>4327</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
@@ -2252,11 +2253,11 @@
       </c>
       <c r="Q22">
         <f t="shared" ca="1" si="12"/>
-        <v>0.26540491412597089</v>
+        <v>0.36473868223062333</v>
       </c>
       <c r="R22">
         <f t="shared" ca="1" si="10"/>
-        <v>2573</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
@@ -2286,11 +2287,11 @@
       </c>
       <c r="Q23">
         <f t="shared" ca="1" si="12"/>
-        <v>0.3488310700022843</v>
+        <v>0.96256201152241105</v>
       </c>
       <c r="R23">
         <f t="shared" ca="1" si="10"/>
-        <v>9384</v>
+        <v>7994</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -2316,11 +2317,11 @@
       </c>
       <c r="Q24">
         <f t="shared" ca="1" si="12"/>
-        <v>0.16303416914360946</v>
+        <v>0.11172218085511543</v>
       </c>
       <c r="R24">
         <f t="shared" ca="1" si="10"/>
-        <v>5968</v>
+        <v>6694</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
@@ -2349,11 +2350,11 @@
       </c>
       <c r="Q25">
         <f t="shared" ca="1" si="12"/>
-        <v>0.85232339580307004</v>
+        <v>0.42031963699898867</v>
       </c>
       <c r="R25">
         <f t="shared" ca="1" si="10"/>
-        <v>9803</v>
+        <v>7186</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
@@ -2378,11 +2379,11 @@
       </c>
       <c r="Q26">
         <f t="shared" ca="1" si="12"/>
-        <v>0.7988890497600476</v>
+        <v>0.77979638702882492</v>
       </c>
       <c r="R26">
         <f t="shared" ca="1" si="10"/>
-        <v>3463</v>
+        <v>6231</v>
       </c>
     </row>
   </sheetData>
@@ -2425,57 +2426,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="33"/>
+      <c r="Y1" s="33"/>
+      <c r="Z1" s="33"/>
+      <c r="AA1" s="33"/>
+      <c r="AB1" s="33"/>
+      <c r="AC1" s="33"/>
     </row>
     <row r="2" spans="1:29" ht="79.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
@@ -3880,13 +3881,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="34" t="s">
         <v>87</v>
       </c>
       <c r="D1" s="7" t="s">
@@ -3933,9 +3934,9 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="7" t="s">
         <v>99</v>
       </c>
@@ -3980,9 +3981,9 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="67.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="9" t="s">
         <v>110</v>
       </c>
@@ -4404,382 +4405,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="33" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-    </row>
-    <row r="2" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C4" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C5" s="3">
-        <f>DATE(2020,12,10)</f>
-        <v>44175</v>
-      </c>
-      <c r="D5" s="3">
-        <f ca="1">TODAY()</f>
-        <v>45701</v>
-      </c>
-      <c r="E5" s="4">
-        <f ca="1">NOW()</f>
-        <v>45701.494058564815</v>
-      </c>
-      <c r="F5" s="5">
-        <f>TIME(2,30,30)</f>
-        <v>0.10451388888888889</v>
-      </c>
-      <c r="G5">
-        <f ca="1">DATEDIF(C5,D5,"ym")</f>
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <f ca="1">YEAR(D5)</f>
-        <v>2025</v>
-      </c>
-      <c r="I5">
-        <f ca="1">DAY(D5)</f>
-        <v>13</v>
-      </c>
-      <c r="J5">
-        <f ca="1">HOUR(E5)</f>
-        <v>11</v>
-      </c>
-      <c r="K5">
-        <f ca="1">MINUTE(E5)</f>
-        <v>51</v>
-      </c>
-      <c r="L5">
-        <f ca="1">SECOND(E5)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I9" s="20">
-        <v>12</v>
-      </c>
-      <c r="J9">
-        <v>12</v>
-      </c>
-      <c r="K9">
-        <v>2002</v>
-      </c>
-      <c r="L9" s="3">
-        <f>DATE(K9,J9,I9)</f>
-        <v>37602</v>
-      </c>
-      <c r="N9" s="3">
-        <v>37602</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="D10" s="3">
-        <f ca="1">TODAY()</f>
-        <v>45701</v>
-      </c>
-      <c r="E10">
-        <f ca="1">YEAR(D10)</f>
-        <v>2025</v>
-      </c>
-      <c r="F10">
-        <f ca="1">MONTH(E10)</f>
-        <v>7</v>
-      </c>
-      <c r="G10">
-        <f ca="1">YEARFRAC(TODAY(),C5)</f>
-        <v>4.1749999999999998</v>
-      </c>
-      <c r="I10" s="20">
-        <v>12</v>
-      </c>
-      <c r="J10">
-        <v>12</v>
-      </c>
-      <c r="K10">
-        <v>2001</v>
-      </c>
-      <c r="L10" s="3">
-        <f t="shared" ref="L10:L18" si="0">DATE(K10,J10,I10)</f>
-        <v>37237</v>
-      </c>
-      <c r="N10" s="3">
-        <v>37237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="D11" s="4">
-        <f ca="1">NOW()</f>
-        <v>45701.494058564815</v>
-      </c>
-      <c r="I11" s="20">
-        <v>12</v>
-      </c>
-      <c r="J11">
-        <v>12</v>
-      </c>
-      <c r="K11">
-        <v>2001</v>
-      </c>
-      <c r="L11" s="3">
-        <f t="shared" si="0"/>
-        <v>37237</v>
-      </c>
-      <c r="M11">
-        <f>DATEDIF(L11,L13,"Y")</f>
-        <v>800</v>
-      </c>
-      <c r="N11" s="3">
-        <v>37237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="I12" s="20"/>
-      <c r="L12" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N12" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E13" s="19">
-        <v>0.61597222222222225</v>
-      </c>
-      <c r="G13" s="4">
-        <v>45695.616666666669</v>
-      </c>
-      <c r="I13" s="20">
-        <v>12</v>
-      </c>
-      <c r="J13">
-        <v>12</v>
-      </c>
-      <c r="K13">
-        <v>2801</v>
-      </c>
-      <c r="L13" s="3">
-        <f>DATE(K13,J13,I13)</f>
-        <v>329431</v>
-      </c>
-      <c r="N13" s="3">
-        <v>329431</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E14" s="3">
-        <f ca="1">TODAY()</f>
-        <v>45701</v>
-      </c>
-      <c r="I14" s="20"/>
-      <c r="L14" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N14" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E15" s="3">
-        <v>45695</v>
-      </c>
-      <c r="G15" s="4">
-        <f ca="1">NOW()</f>
-        <v>45701.494058564815</v>
-      </c>
-      <c r="I15" s="20">
-        <v>12</v>
-      </c>
-      <c r="J15">
-        <v>12</v>
-      </c>
-      <c r="K15">
-        <v>2009</v>
-      </c>
-      <c r="L15" s="3">
-        <f>DATE(K15,J15,I15)</f>
-        <v>40159</v>
-      </c>
-      <c r="N15" s="3">
-        <v>40159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="E16" s="19">
-        <v>0.61597222222222225</v>
-      </c>
-      <c r="I16" s="20"/>
-      <c r="L16" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N16" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="I17" s="20"/>
-      <c r="L17" s="3" t="e">
-        <f t="shared" si="0"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="N17" s="3" t="e">
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E18" s="3">
-        <v>45695</v>
-      </c>
-      <c r="I18" s="20">
-        <v>12</v>
-      </c>
-      <c r="J18">
-        <v>12</v>
-      </c>
-      <c r="K18">
-        <v>2001</v>
-      </c>
-      <c r="L18" s="3">
-        <f t="shared" si="0"/>
-        <v>37237</v>
-      </c>
-      <c r="N18" s="3">
-        <v>37237</v>
-      </c>
-    </row>
-    <row r="19" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E19" s="19">
-        <v>0.61597222222222225</v>
-      </c>
-      <c r="L19" t="s">
-        <v>136</v>
-      </c>
-      <c r="N19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
-      <c r="E20" s="19">
-        <v>0.6166666666666667</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="G2:N2"/>
-    <mergeCell ref="A1:T1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.21875" customWidth="1"/>
-    <col min="10" max="10" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
-        <v>138</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -4800,22 +4427,23 @@
       <c r="R1" s="33"/>
       <c r="S1" s="33"/>
       <c r="T1" s="33"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+    </row>
+    <row r="2" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="32" t="s">
+        <v>59</v>
+      </c>
       <c r="H2" s="32"/>
       <c r="I2" s="32"/>
       <c r="J2" s="32"/>
@@ -4823,13 +4451,386 @@
       <c r="L2" s="32"/>
       <c r="M2" s="32"/>
       <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C5" s="3">
+        <f>DATE(2020,12,10)</f>
+        <v>44175</v>
+      </c>
+      <c r="D5" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45701</v>
+      </c>
+      <c r="E5" s="4">
+        <f ca="1">NOW()</f>
+        <v>45701.618897800923</v>
+      </c>
+      <c r="F5" s="5">
+        <f>TIME(2,30,30)</f>
+        <v>0.10451388888888889</v>
+      </c>
+      <c r="G5">
+        <f ca="1">DATEDIF(C5,D5,"ym")</f>
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <f ca="1">YEAR(D5)</f>
+        <v>2025</v>
+      </c>
+      <c r="I5">
+        <f ca="1">DAY(D5)</f>
+        <v>13</v>
+      </c>
+      <c r="J5">
+        <f ca="1">HOUR(E5)</f>
+        <v>14</v>
+      </c>
+      <c r="K5">
+        <f ca="1">MINUTE(E5)</f>
+        <v>51</v>
+      </c>
+      <c r="L5">
+        <f ca="1">SECOND(E5)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I9" s="20">
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+      <c r="K9">
+        <v>2002</v>
+      </c>
+      <c r="L9" s="3">
+        <f>DATE(K9,J9,I9)</f>
+        <v>37602</v>
+      </c>
+      <c r="N9" s="3">
+        <v>37602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D10" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45701</v>
+      </c>
+      <c r="E10">
+        <f ca="1">YEAR(D10)</f>
+        <v>2025</v>
+      </c>
+      <c r="F10">
+        <f ca="1">MONTH(E10)</f>
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <f ca="1">YEARFRAC(TODAY(),C5)</f>
+        <v>4.1749999999999998</v>
+      </c>
+      <c r="I10" s="20">
+        <v>12</v>
+      </c>
+      <c r="J10">
+        <v>12</v>
+      </c>
+      <c r="K10">
+        <v>2001</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" ref="L10:L18" si="0">DATE(K10,J10,I10)</f>
+        <v>37237</v>
+      </c>
+      <c r="N10" s="3">
+        <v>37237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="D11" s="4">
+        <f ca="1">NOW()</f>
+        <v>45701.618897685184</v>
+      </c>
+      <c r="I11" s="20">
+        <v>12</v>
+      </c>
+      <c r="J11">
+        <v>12</v>
+      </c>
+      <c r="K11">
+        <v>2001</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="0"/>
+        <v>37237</v>
+      </c>
+      <c r="M11">
+        <f>DATEDIF(L11,L13,"Y")</f>
+        <v>800</v>
+      </c>
+      <c r="N11" s="3">
+        <v>37237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="I12" s="20"/>
+      <c r="L12" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N12" s="3" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="E13" s="19">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="G13" s="4">
+        <v>45695.616666666669</v>
+      </c>
+      <c r="I13" s="20">
+        <v>12</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>2801</v>
+      </c>
+      <c r="L13" s="3">
+        <f>DATE(K13,J13,I13)</f>
+        <v>329431</v>
+      </c>
+      <c r="N13" s="3">
+        <v>329431</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="E14" s="3">
+        <f ca="1">TODAY()</f>
+        <v>45701</v>
+      </c>
+      <c r="I14" s="20"/>
+      <c r="L14" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N14" s="3" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="E15" s="3">
+        <v>45695</v>
+      </c>
+      <c r="G15" s="4">
+        <f ca="1">NOW()</f>
+        <v>45701.618897685184</v>
+      </c>
+      <c r="I15" s="20">
+        <v>12</v>
+      </c>
+      <c r="J15">
+        <v>12</v>
+      </c>
+      <c r="K15">
+        <v>2009</v>
+      </c>
+      <c r="L15" s="3">
+        <f>DATE(K15,J15,I15)</f>
+        <v>40159</v>
+      </c>
+      <c r="N15" s="3">
+        <v>40159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="E16" s="19">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="I16" s="20"/>
+      <c r="L16" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N16" s="3" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="I17" s="20"/>
+      <c r="L17" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="N17" s="3" t="e">
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E18" s="3">
+        <v>45695</v>
+      </c>
+      <c r="I18" s="20">
+        <v>12</v>
+      </c>
+      <c r="J18">
+        <v>12</v>
+      </c>
+      <c r="K18">
+        <v>2001</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" si="0"/>
+        <v>37237</v>
+      </c>
+      <c r="N18" s="3">
+        <v>37237</v>
+      </c>
+    </row>
+    <row r="19" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E19" s="19">
+        <v>0.61597222222222225</v>
+      </c>
+      <c r="L19" t="s">
+        <v>136</v>
+      </c>
+      <c r="N19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E20" s="19">
+        <v>0.6166666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G2:N2"/>
+    <mergeCell ref="A1:T1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.21875" customWidth="1"/>
+    <col min="10" max="10" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="21"/>
       <c r="E3" s="21"/>
       <c r="F3" s="21"/>
@@ -4845,9 +4846,9 @@
       <c r="P3" s="21"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="23" t="s">
         <v>142</v>
       </c>
@@ -5047,10 +5048,10 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="B16" s="30"/>
+      <c r="B16" s="35"/>
       <c r="C16">
         <v>1</v>
       </c>
@@ -5072,10 +5073,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="B17" s="30"/>
+      <c r="B17" s="35"/>
       <c r="C17">
         <v>1</v>
       </c>
@@ -5117,7 +5118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -5129,51 +5130,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33"/>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
       <c r="O2" s="22"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
@@ -5182,17 +5183,17 @@
       <c r="T2" s="22"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -5426,10 +5427,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C15" sqref="C15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5443,198 +5444,207 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="35" t="s">
         <v>188</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
-      <c r="R3" s="38"/>
-      <c r="S3" s="38"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="31" t="s">
         <v>177</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="31">
         <v>25</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="38">
-        <f>INDEX(A4:B7, 3,2)</f>
+      <c r="D5" s="30">
+        <f>INDEX(A4:C21, 3,2)</f>
         <v>30</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="30">
         <f>MATCH("Sarah", A4:A7, 0)</f>
         <v>3</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="30">
         <f ca="1">INDIRECT("B5")</f>
         <v>25</v>
       </c>
-      <c r="G5" s="38" t="str">
+      <c r="G5" s="30" t="str">
         <f ca="1">OFFSET(B5, 2, 1)</f>
-        <v>sdsfds</v>
-      </c>
-      <c r="H5" s="38" t="str">
+        <v>male</v>
+      </c>
+      <c r="H5" s="30" t="str">
         <f>CHOOSE(2, A5,A6,A7)</f>
         <v>Sarah</v>
       </c>
-      <c r="I5" s="38">
+      <c r="I5" s="30">
         <f>ROW(C7)</f>
         <v>7</v>
       </c>
-      <c r="J5" s="38">
+      <c r="J5" s="30">
         <f>COLUMN(C7)</f>
         <v>3</v>
       </c>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="38"/>
-      <c r="S5" s="38"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+      <c r="S5" s="30"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A6" s="39" t="s">
+      <c r="A6" s="31" t="s">
         <v>178</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="31">
         <v>30</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38">
+      <c r="D6" s="30"/>
+      <c r="E6" s="30">
+        <f>MATCH(27, B4:B7, 1)</f>
+        <v>2</v>
+      </c>
+      <c r="F6" s="30">
         <f>B5</f>
         <v>25</v>
       </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="38"/>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="38"/>
-      <c r="Q6" s="38"/>
-      <c r="R6" s="38"/>
-      <c r="S6" s="38"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+      <c r="S6" s="30"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="34">
+      <c r="B7" s="27">
         <v>35</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="27" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="D15" t="str">
+        <f>A5</f>
+        <v>John</v>
       </c>
     </row>
   </sheetData>
@@ -5645,4 +5655,129 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="str">
+        <f>'Reference Functions'!A4</f>
+        <v>Name</v>
+      </c>
+      <c r="B1" t="str">
+        <f>'Reference Functions'!C4</f>
+        <v>Gender</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="str">
+        <f>'Reference Functions'!A5</f>
+        <v>John</v>
+      </c>
+      <c r="B2" t="str">
+        <f>'Reference Functions'!C5</f>
+        <v>Male</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="str">
+        <f>'Reference Functions'!A6</f>
+        <v>Sarah</v>
+      </c>
+      <c r="B3" t="str">
+        <f>'Reference Functions'!C6</f>
+        <v>Female</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="str">
+        <f>'Reference Functions'!A7</f>
+        <v>Mike</v>
+      </c>
+      <c r="B4" t="str">
+        <f>'Reference Functions'!C7</f>
+        <v>male</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <f>'Reference Functions'!A8</f>
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <f>'Reference Functions'!C8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <f>'Reference Functions'!A9</f>
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <f>'Reference Functions'!C9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f>'Reference Functions'!A10</f>
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <f>'Reference Functions'!C10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>'Reference Functions'!A11</f>
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <f>'Reference Functions'!C11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>'Reference Functions'!A12</f>
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <f>'Reference Functions'!C12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f>'Reference Functions'!A13</f>
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <f>'Reference Functions'!C13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f>'Reference Functions'!A14</f>
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <f>'Reference Functions'!C14</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>